<commit_message>
Redéfinition de la zone imprimable; adapt Gros oeuvre
</commit_message>
<xml_diff>
--- a/planning/JVE_Planning.xlsx
+++ b/planning/JVE_Planning.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\workspace\perso\maison\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\maison\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD85EA32-B1AF-4A61-8F38-18E9F0016E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="664"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -17,13 +18,13 @@
     <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Dashboard!$A$1:$X$46</definedName>
     <definedName name="Slicer_Manager">#N/A</definedName>
     <definedName name="Slicer_Project">#N/A</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Dashboard!$A:$AX</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -390,7 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0\ &quot;Days&quot;"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -631,7 +632,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="74">
     <dxf>
@@ -1128,7 +1129,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="No Border" pivot="0" table="0" count="10">
+    <tableStyle name="No Border" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="73"/>
       <tableStyleElement type="headerRow" dxfId="72"/>
     </tableStyle>
@@ -1401,7 +1402,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1538,7 +1539,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1546,6 +1546,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -1577,7 +1578,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2435,7 +2436,6 @@
         </c:spPr>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2481,7 +2481,6 @@
                   <a:avLst/>
                 </a:prstGeom>
               </c15:spPr>
-              <c15:layout/>
             </c:ext>
           </c:extLst>
         </c:dLbl>
@@ -2671,7 +2670,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -2682,9 +2680,7 @@
               <c:separator>
 </c:separator>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-3E89-438F-9816-332D1E0E14DC}"/>
                 </c:ext>
@@ -2769,7 +2765,7 @@
             <c:numRef>
               <c:f>Workings!$B$3</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0,,"M"</c:formatCode>
+                <c:formatCode>#\ ##0.0\ \ "M"</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>39582.17</c:v>
@@ -2952,7 +2948,7 @@
             <c:numRef>
               <c:f>Workings!$C$3</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0,,"M"</c:formatCode>
+                <c:formatCode>#\ ##0.0\ \ "M"</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>261504.37</c:v>
@@ -3005,7 +3001,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="#,##0.0,,&quot;M&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.0\ \ &quot;M&quot;" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3023,7 +3019,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3031,6 +3026,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -3075,7 +3071,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3229,7 +3225,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3329,7 +3324,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3436,7 +3430,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3571,7 +3564,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3579,6 +3571,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -3609,7 +3602,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3784,7 +3777,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3792,6 +3784,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -4949,7 +4942,7 @@
             <xdr:cNvPr id="8" name="Manager">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5027,7 +5020,7 @@
             <xdr:cNvPr id="3" name="Project">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5103,7 +5096,7 @@
         <xdr:cNvPr id="14" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5141,7 +5134,7 @@
         <xdr:cNvPr id="18" name="Chart 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5184,7 +5177,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5229,7 +5222,7 @@
         <xdr:cNvPr id="19" name="Chart 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5267,7 +5260,7 @@
         <xdr:cNvPr id="20" name="Chart 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5305,7 +5298,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5670,7 +5663,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jean-Marc VERLAINE" refreshedDate="44439.501697916668" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jean-Marc VERLAINE" refreshedDate="44439.501697916668" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48" xr:uid="{00000000-000A-0000-FFFF-FFFF0A000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -6478,7 +6471,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Gantt" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="Gantt" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A5:J54" firstHeaderRow="0" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="10">
     <pivotField name="Topic" axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -7370,91 +7363,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Days_Completed" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0">
-      <items count="17">
-        <item x="12"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="16">
-        <item x="8"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" numFmtId="3" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField numFmtId="3" showAll="0"/>
-    <pivotField numFmtId="3" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Days completed " fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Duration " fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Budget_v_Actual" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Budget_v_Actual" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="B2:C3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="10">
     <pivotField showAll="0">
@@ -7602,8 +7511,92 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="Days_Completed" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0">
+      <items count="17">
+        <item x="12"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="16">
+        <item x="8"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Days completed " fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Duration " fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Project" sourceName="Project">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Project" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="Project">
   <pivotTables>
     <pivotTable tabId="3" name="Gantt"/>
     <pivotTable tabId="4" name="Days_Completed"/>
@@ -7635,7 +7628,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Manager" sourceName="Manager">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Manager" xr10:uid="{00000000-0013-0000-FFFF-FFFF02000000}" sourceName="Manager">
   <pivotTables>
     <pivotTable tabId="3" name="Gantt"/>
     <pivotTable tabId="4" name="Budget_v_Actual"/>
@@ -7666,30 +7659,30 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Project" cache="Slicer_Project" caption="Topic" columnCount="5" style="SlicerStyleLight2" rowHeight="252000"/>
-  <slicer name="Manager" cache="Slicer_Manager" caption="Acteur" columnCount="5" style="SlicerStyleLight2" rowHeight="252000"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Project" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="Slicer_Project" caption="Topic" columnCount="5" style="SlicerStyleLight2" rowHeight="252000"/>
+  <slicer name="Manager" xr10:uid="{00000000-0014-0000-FFFF-FFFF02000000}" cache="Slicer_Manager" caption="Acteur" columnCount="5" style="SlicerStyleLight2" rowHeight="252000"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J49" totalsRowShown="0">
-  <autoFilter ref="A1:J49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J49" totalsRowShown="0">
+  <autoFilter ref="A1:J49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Project"/>
-    <tableColumn id="2" name="Task"/>
-    <tableColumn id="3" name="Manager"/>
-    <tableColumn id="4" name="Start Date" dataDxfId="5"/>
-    <tableColumn id="5" name="Duration"/>
-    <tableColumn id="9" name="End Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Project"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Manager"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Start Date" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Duration"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="End Date" dataDxfId="4">
       <calculatedColumnFormula>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Days completed" dataDxfId="3"/>
-    <tableColumn id="6" name="Progress" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Days completed" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Progress" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Days completed]]/Table1[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Budget" dataDxfId="1"/>
-    <tableColumn id="8" name="Actual" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Budget" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Actual" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7991,18 +7984,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BA85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -8026,7 +8019,7 @@
       <c r="B1" s="26"/>
       <c r="C1" s="46" t="str">
         <f>TEXT(MIN(D6:D51),"d-mmm-yy")&amp;" to "&amp;TEXT(MAX(E6:E51),"d-mmm-yy")</f>
-        <v>23-Apr-21 to 23-Mar-22</v>
+        <v>d-avr-yy to d-mars-yy</v>
       </c>
       <c r="D1" s="46"/>
       <c r="E1" s="46"/>
@@ -10283,7 +10276,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.14000000000000001" right="0.12" top="0.3" bottom="0.12" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="64" fitToWidth="0" orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10340,7 +10333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -10348,7 +10341,7 @@
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.5703125" customWidth="1"/>
@@ -10404,7 +10397,7 @@
       </c>
       <c r="G2" s="5" t="str">
         <f ca="1">_xlfn.FORMULATEXT(F2)</f>
-        <v>=COUNTIF(Dashboard!H6:H51,"="&amp;0)</v>
+        <v>=NB.SI(Dashboard!H6:H51;"="&amp;0)</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -10441,7 +10434,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f ca="1">_xlfn.FORMULATEXT(F3)</f>
-        <v>=COUNTIFS(Dashboard!H6:H51,"&lt;&gt;"&amp;0,Dashboard!H6:H51,"&lt;"&amp;1)</v>
+        <v>=NB.SI.ENS(Dashboard!H6:H51;"&lt;&gt;"&amp;0;Dashboard!H6:H51;"&lt;"&amp;1)</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>22</v>
@@ -10483,7 +10476,7 @@
       </c>
       <c r="G4" s="5" t="str">
         <f ca="1">_xlfn.FORMULATEXT(F4)</f>
-        <v>=COUNTIF(Dashboard!H6:H51,"="&amp;1)</v>
+        <v>=NB.SI(Dashboard!H6:H51;"="&amp;1)</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>27</v>
@@ -10535,7 +10528,7 @@
       </c>
       <c r="G6" s="5" t="str">
         <f ca="1">_xlfn.FORMULATEXT(F6)</f>
-        <v>=COUNTA(Dashboard!B6:B50)</v>
+        <v>=NBVAL(Dashboard!B6:B50)</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -10552,15 +10545,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
@@ -10687,14 +10680,14 @@
         <v>36</v>
       </c>
       <c r="D4" s="1">
-        <v>44445</v>
+        <v>44447</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
         <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>44446</v>
+        <v>44449</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -10722,14 +10715,14 @@
         <v>36</v>
       </c>
       <c r="D5" s="1">
-        <v>44442</v>
+        <v>44448</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="1">
         <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>44442</v>
+        <v>44448</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -10756,14 +10749,14 @@
         <v>36</v>
       </c>
       <c r="D6" s="1">
-        <v>44439</v>
+        <v>44445</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="1">
         <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>44439</v>
+        <v>44445</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -10793,18 +10786,18 @@
         <v>44438</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1">
         <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="2">
         <f>Table1[[#This Row],[Days completed]]/Table1[[#This Row],[Duration]]</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I7" s="41">
         <v>5088</v>

</xml_diff>